<commit_message>
se hizo p12 y p13, ademas lo que tiene que ver con el examen
</commit_message>
<xml_diff>
--- a/Estructura_de_datos/src/Media/Archivos/datose1_2024_1E.xlsx
+++ b/Estructura_de_datos/src/Media/Archivos/datose1_2024_1E.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3e8f32763bd0572d/Documentos/Mis_docs/4toSemestre/Estructura-Datos/ED_4B_2025/src/Media/Archivos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3e8f32763bd0572d/Documentos/Estructura-Datos/Estructura-Datos/Estructura_de_datos/src/Media/Archivos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="11_D995EE5E94AECA0550248A571CBF6024A6419338" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{884890AA-2CE0-4B3A-A549-8BC88C5E27DB}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="11_D995EE5E94AECA0550248A571CBF6024A6419338" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{844726E5-E6C6-48EA-ACAB-8CB246BC71A2}"/>
   <bookViews>
     <workbookView minimized="1" xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,10 +17,21 @@
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -94,6 +105,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -385,8 +400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E498"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="E439" sqref="E439"/>
+    <sheetView tabSelected="1" topLeftCell="A488" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="A500" sqref="A500"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>